<commit_message>
ITSADSSD-21749 - Amend vevo check file
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Manish Gupta\UiPath_Projects\FrameworkExcelAsInput\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmgupt1\Documents\UiPath\RpaUiPathProcess\Processes\PBI_LocationCheck\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -152,12 +152,6 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
@@ -167,17 +161,47 @@
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>InputList</t>
-  </si>
-  <si>
-    <t>Data/Input/Test1.csv</t>
+    <t>CSVFolder_Location</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>SSO_rpa00001</t>
+  </si>
+  <si>
+    <t>EmailExchangeServer</t>
+  </si>
+  <si>
+    <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>NumberOfEmails</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck_SenderEmail</t>
+  </si>
+  <si>
+    <t>IAA_Vevo_ImmiAccount</t>
+  </si>
+  <si>
+    <t>Subject_Prefix</t>
+  </si>
+  <si>
+    <t>Location VEVO check</t>
+  </si>
+  <si>
+    <t>Immi_Website</t>
+  </si>
+  <si>
+    <t>https://online.immi.gov.au/lusc/login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -187,6 +211,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -207,14 +237,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,7 +566,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -575,39 +611,60 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1596,6 +1653,10 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1605,7 +1666,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D17"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2816,9 +2877,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2859,9 +2922,30 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3858,6 +3942,7 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ITSADSSD-21887 -  Placeholder for git and code changes for send email
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -155,15 +155,9 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
   <si>
-    <t>CSVFolder_Location</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -195,6 +189,63 @@
   </si>
   <si>
     <t>https://online.immi.gov.au/lusc/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to save input file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange server web address to retrive emails </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
+  </si>
+  <si>
+    <t>Subject for email received from PBI team ro perform check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to move email after processing </t>
+  </si>
+  <si>
+    <t>PBI_Archive</t>
+  </si>
+  <si>
+    <t>Credentials for SSO account  RPA00001</t>
+  </si>
+  <si>
+    <t>Credentials for Immi website login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI team email address </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>UQ SMTP server address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ SMTP port number </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck</t>
+  </si>
+  <si>
+    <t>FolderName</t>
+  </si>
+  <si>
+    <t>Folder_Location</t>
+  </si>
+  <si>
+    <t>File_Name</t>
+  </si>
+  <si>
+    <t>EXTRACT_FOR_ROBOT.csv</t>
+  </si>
+  <si>
+    <t>File name for input, received from PBI team</t>
   </si>
 </sst>
 </file>
@@ -563,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -614,59 +665,91 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="3">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1652,10 +1735,12 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2879,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2924,30 +3009,59 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-21751 - Changes to Send Email
To save a copy of email in sent item
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -188,64 +188,115 @@
     <t>Immi_Website</t>
   </si>
   <si>
+    <t xml:space="preserve">Folder to save input file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange server web address to retrive emails </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
+  </si>
+  <si>
+    <t>Subject for email received from PBI team ro perform check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to move email after processing </t>
+  </si>
+  <si>
+    <t>Credentials for SSO account  RPA00001</t>
+  </si>
+  <si>
+    <t>Credentials for Immi website login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI team email address </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>UQ SMTP server address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UQ SMTP port number </t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck</t>
+  </si>
+  <si>
+    <t>Folder_Location</t>
+  </si>
+  <si>
+    <t>File_Name</t>
+  </si>
+  <si>
+    <t>EXTRACT_FOR_ROBOT.csv</t>
+  </si>
+  <si>
+    <t>File name for input, received from PBI team</t>
+  </si>
+  <si>
+    <t>Archive_Folder</t>
+  </si>
+  <si>
+    <t>PBI_Archive</t>
+  </si>
+  <si>
+    <t>Immi website (extrenal url)</t>
+  </si>
+  <si>
     <t>https://online.immi.gov.au/lusc/login</t>
   </si>
   <si>
-    <t xml:space="preserve">Folder to save input file </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange server web address to retrive emails </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
-  </si>
-  <si>
-    <t>Subject for email received from PBI team ro perform check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder to move email after processing </t>
-  </si>
-  <si>
-    <t>PBI_Archive</t>
-  </si>
-  <si>
-    <t>Credentials for SSO account  RPA00001</t>
-  </si>
-  <si>
-    <t>Credentials for Immi website login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBI team email address </t>
-  </si>
-  <si>
-    <t>UQ_SMTP_SERVER</t>
-  </si>
-  <si>
-    <t>UQ SMTP server address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UQ SMTP port number </t>
-  </si>
-  <si>
-    <t>UQ_SMTP_PORT</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck</t>
-  </si>
-  <si>
-    <t>FolderName</t>
-  </si>
-  <si>
-    <t>Folder_Location</t>
-  </si>
-  <si>
-    <t>File_Name</t>
-  </si>
-  <si>
-    <t>EXTRACT_FOR_ROBOT.csv</t>
-  </si>
-  <si>
-    <t>File name for input, received from PBI team</t>
+    <t>Email_MessageBody</t>
+  </si>
+  <si>
+    <t>Email message body for response email</t>
+  </si>
+  <si>
+    <t>Email_SenderName</t>
+  </si>
+  <si>
+    <t>PBI-LocationCheck Bot</t>
+  </si>
+  <si>
+    <t>Email_SenderAddress</t>
+  </si>
+  <si>
+    <t>rpa00001@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Email_AlertRecipient</t>
+  </si>
+  <si>
+    <t>rpa.ads@its.uq.edu.au</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi Team, Please find VEVO location check result attached. There are {0} records processed. Thanks, RPA Bot </t>
+  </si>
+  <si>
+    <t>Sender name on email</t>
+  </si>
+  <si>
+    <t>Sender email address</t>
+  </si>
+  <si>
+    <t>Email_Alert_MessageBody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention Team – PBI_LocationCheck process the records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body for move message to archive folder error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPA ADS support email address </t>
+  </si>
+  <si>
+    <t>Email_Alert_Subject</t>
   </si>
 </sst>
 </file>
@@ -616,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -665,24 +716,24 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,7 +741,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
@@ -705,7 +756,7 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -716,7 +767,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -727,18 +778,18 @@
         <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -747,7 +798,10 @@
         <v>54</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1748,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1979,12 +2033,67 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2955,7 +3064,12 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1"/>
+    <hyperlink ref="B28" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2964,7 +3078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3015,7 +3129,7 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3026,7 +3140,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3037,29 +3151,29 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-21811 - Changes to add quotes in output file and error handling
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -167,136 +167,136 @@
     <t>EmailExchangeServer</t>
   </si>
   <si>
+    <t>NumberOfEmails</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck_SenderEmail</t>
+  </si>
+  <si>
+    <t>IAA_Vevo_ImmiAccount</t>
+  </si>
+  <si>
+    <t>Subject_Prefix</t>
+  </si>
+  <si>
+    <t>Location VEVO check</t>
+  </si>
+  <si>
+    <t>Immi_Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to save input file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange server web address to retrive emails </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
+  </si>
+  <si>
+    <t>Subject for email received from PBI team ro perform check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to move email after processing </t>
+  </si>
+  <si>
+    <t>Credentials for SSO account  RPA00001</t>
+  </si>
+  <si>
+    <t>Credentials for Immi website login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI team email address </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck</t>
+  </si>
+  <si>
+    <t>Folder_Location</t>
+  </si>
+  <si>
+    <t>File_Name</t>
+  </si>
+  <si>
+    <t>EXTRACT_FOR_ROBOT.csv</t>
+  </si>
+  <si>
+    <t>File name for input, received from PBI team</t>
+  </si>
+  <si>
+    <t>Archive_Folder</t>
+  </si>
+  <si>
+    <t>PBI_Archive</t>
+  </si>
+  <si>
+    <t>Immi website (extrenal url)</t>
+  </si>
+  <si>
+    <t>Email_MessageBody</t>
+  </si>
+  <si>
+    <t>Email message body for response email</t>
+  </si>
+  <si>
+    <t>Email_AlertRecipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body for move message to archive folder error. </t>
+  </si>
+  <si>
+    <t>Email_Alert_Subject</t>
+  </si>
+  <si>
+    <t>EmailMsg_MoveFolder</t>
+  </si>
+  <si>
+    <t>EmailMsg_InitError</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck - Error Notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - PBI_LocationCheck process the records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention - PBI_LocationCheck encounter error during Initialization with following error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please find VEVO location check result attached. There are {0} records processed. </t>
+  </si>
+  <si>
+    <t>https://online.immi.gov.au/lusc/login</t>
+  </si>
+  <si>
     <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
   </si>
   <si>
-    <t>NumberOfEmails</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck_SenderEmail</t>
-  </si>
-  <si>
-    <t>IAA_Vevo_ImmiAccount</t>
-  </si>
-  <si>
-    <t>Subject_Prefix</t>
-  </si>
-  <si>
-    <t>Location VEVO check</t>
-  </si>
-  <si>
-    <t>Immi_Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder to save input file </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange server web address to retrive emails </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
-  </si>
-  <si>
-    <t>Subject for email received from PBI team ro perform check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder to move email after processing </t>
-  </si>
-  <si>
-    <t>Credentials for SSO account  RPA00001</t>
-  </si>
-  <si>
-    <t>Credentials for Immi website login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBI team email address </t>
-  </si>
-  <si>
-    <t>UQ_SMTP_SERVER</t>
-  </si>
-  <si>
-    <t>UQ SMTP server address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UQ SMTP port number </t>
-  </si>
-  <si>
-    <t>UQ_SMTP_PORT</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck</t>
-  </si>
-  <si>
-    <t>Folder_Location</t>
-  </si>
-  <si>
-    <t>File_Name</t>
-  </si>
-  <si>
-    <t>EXTRACT_FOR_ROBOT.csv</t>
-  </si>
-  <si>
-    <t>File name for input, received from PBI team</t>
-  </si>
-  <si>
-    <t>Archive_Folder</t>
-  </si>
-  <si>
-    <t>PBI_Archive</t>
-  </si>
-  <si>
-    <t>Immi website (extrenal url)</t>
-  </si>
-  <si>
-    <t>https://online.immi.gov.au/lusc/login</t>
-  </si>
-  <si>
-    <t>Email_MessageBody</t>
-  </si>
-  <si>
-    <t>Email message body for response email</t>
-  </si>
-  <si>
-    <t>Email_SenderName</t>
-  </si>
-  <si>
-    <t>PBI-LocationCheck Bot</t>
-  </si>
-  <si>
-    <t>Email_SenderAddress</t>
-  </si>
-  <si>
-    <t>rpa00001@uq.edu.au</t>
-  </si>
-  <si>
-    <t>Email_AlertRecipient</t>
+    <t>Output_Header</t>
+  </si>
+  <si>
+    <t>EMPLID,FAMILY_NAME,GIVEN_NAMES,BIRTH_DATE,PASSPORT_NUMBER,PASSPORT_COUNTRY,LOCATION,UPDATETIMESTAMP,ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header fields for output file </t>
   </si>
   <si>
     <t>rpa.ads@its.uq.edu.au</t>
   </si>
   <si>
-    <t xml:space="preserve">Hi Team, Please find VEVO location check result attached. There are {0} records processed. Thanks, RPA Bot </t>
-  </si>
-  <si>
-    <t>Sender name on email</t>
-  </si>
-  <si>
-    <t>Sender email address</t>
-  </si>
-  <si>
-    <t>Email_Alert_MessageBody</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attention Team – PBI_LocationCheck process the records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email message body for move message to archive folder error. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPA ADS support email address </t>
-  </si>
-  <si>
-    <t>Email_Alert_Subject</t>
+    <t xml:space="preserve">RPA ADS support email address   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email subject for error notification. </t>
+  </si>
+  <si>
+    <t>NoEmail_Message</t>
+  </si>
+  <si>
+    <t>Error message if no email or attachment found in mailbox</t>
+  </si>
+  <si>
+    <t>No new email or attachment found in mailbox to process.</t>
   </si>
 </sst>
 </file>
@@ -665,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -716,95 +716,105 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="3">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="3">
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1791,10 +1801,11 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1802,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2035,63 +2046,65 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3064,11 +3077,9 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1"/>
-    <hyperlink ref="B28" r:id="rId2"/>
+    <hyperlink ref="B27" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3079,7 +3090,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3129,53 +3140,33 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-21751 - Append environment name in subject line for NonProd env
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -257,9 +257,6 @@
     <t>PBI_LocationCheck - Error Notification</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention - PBI_LocationCheck process the records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Attention - PBI_LocationCheck encounter error during Initialization with following error. </t>
   </si>
   <si>
@@ -281,22 +278,31 @@
     <t xml:space="preserve">Header fields for output file </t>
   </si>
   <si>
+    <t xml:space="preserve">Email subject for error notification. </t>
+  </si>
+  <si>
+    <t>NoEmail_Message</t>
+  </si>
+  <si>
+    <t>Error message if no email or attachment found in mailbox</t>
+  </si>
+  <si>
+    <t>No new email or attachment found in mailbox to process.</t>
+  </si>
+  <si>
+    <t>OperatingEnvironment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot running environment </t>
+  </si>
+  <si>
+    <t>RPA ADS support email address   -</t>
+  </si>
+  <si>
     <t>rpa.ads@its.uq.edu.au</t>
   </si>
   <si>
-    <t xml:space="preserve">RPA ADS support email address   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email subject for error notification. </t>
-  </si>
-  <si>
-    <t>NoEmail_Message</t>
-  </si>
-  <si>
-    <t>Error message if no email or attachment found in mailbox</t>
-  </si>
-  <si>
-    <t>No new email or attachment found in mailbox to process.</t>
+    <t xml:space="preserve">Attention - PBI_LocationCheck process all records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
   </si>
 </sst>
 </file>
@@ -738,13 +744,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>84</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,7 +770,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
         <v>55</v>
@@ -809,7 +815,7 @@
         <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>69</v>
@@ -1816,7 +1822,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2046,13 +2052,13 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2060,7 +2066,7 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -2071,10 +2077,10 @@
         <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2085,7 +2091,7 @@
         <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,7 +2099,7 @@
         <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
         <v>73</v>
@@ -2104,7 +2110,7 @@
         <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3090,7 +3096,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3165,7 +3171,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-22117 - Changes to move mail to archive folder if no attachment
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Email_AlertRecipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Email message body for move message to archive folder error. </t>
-  </si>
-  <si>
     <t>Email_Alert_Subject</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>PBI_LocationCheck - Error Notification</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention - PBI_LocationCheck encounter error during Initialization with following error. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Please find VEVO location check result attached. There are {0} records processed. </t>
   </si>
   <si>
@@ -296,13 +290,49 @@
     <t xml:space="preserve">Robot running environment </t>
   </si>
   <si>
+    <t>EmailMsg_InvalidCSV</t>
+  </si>
+  <si>
+    <t>Email message body if initialization error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message if move message to archive folder encounter error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if move invalid email (no attachment) to archive folder encounter error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if error encountred while trying to read input CSV. </t>
+  </si>
+  <si>
+    <t>EmailMsg_InvalidEmail_MoveFolder</t>
+  </si>
+  <si>
+    <t>EmailMsg_NoAttachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if no input csv attached to email </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error during Initialization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI_LocationCheck process all records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error while trying to move email to archive folder.</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error while trying to read input csv file.</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck process unable to process as bot didn't find input csv file 'EXTRACT_FOR_ROBOT.csv' in attachement.</t>
+  </si>
+  <si>
     <t>RPA ADS support email address   -</t>
   </si>
   <si>
     <t>rpa.ads@its.uq.edu.au</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attention - PBI_LocationCheck process all records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
   </si>
 </sst>
 </file>
@@ -674,7 +704,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -744,13 +774,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,7 +800,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>55</v>
@@ -815,7 +845,7 @@
         <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>69</v>
@@ -1822,7 +1852,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2052,13 +2082,13 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
-        <v>88</v>
-      </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,7 +2096,7 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>71</v>
@@ -2077,60 +2107,93 @@
         <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3096,7 +3159,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3173,13 +3236,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ITSADSSD-22165 -  For non-prod, include environment in subject
For non-prod, include environment in subject and change asset to contain multiple email address
</commit_message>
<xml_diff>
--- a/Processes/PBI_LocationCheck/Data/Config.xlsx
+++ b/Processes/PBI_LocationCheck/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
     <t>Name</t>
   </si>
@@ -179,160 +179,163 @@
     <t>Subject_Prefix</t>
   </si>
   <si>
+    <t>Immi_Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to save input file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange server web address to retrive emails </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
+  </si>
+  <si>
+    <t>Subject for email received from PBI team ro perform check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folder to move email after processing </t>
+  </si>
+  <si>
+    <t>Credentials for SSO account  RPA00001</t>
+  </si>
+  <si>
+    <t>Credentials for Immi website login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI team email address </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck</t>
+  </si>
+  <si>
+    <t>Folder_Location</t>
+  </si>
+  <si>
+    <t>File_Name</t>
+  </si>
+  <si>
+    <t>EXTRACT_FOR_ROBOT.csv</t>
+  </si>
+  <si>
+    <t>File name for input, received from PBI team</t>
+  </si>
+  <si>
+    <t>Archive_Folder</t>
+  </si>
+  <si>
+    <t>PBI_Archive</t>
+  </si>
+  <si>
+    <t>Immi website (extrenal url)</t>
+  </si>
+  <si>
+    <t>Email_MessageBody</t>
+  </si>
+  <si>
+    <t>Email message body for response email</t>
+  </si>
+  <si>
+    <t>Email_AlertRecipient</t>
+  </si>
+  <si>
+    <t>Email_Alert_Subject</t>
+  </si>
+  <si>
+    <t>EmailMsg_MoveFolder</t>
+  </si>
+  <si>
+    <t>EmailMsg_InitError</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck - Error Notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please find VEVO location check result attached. There are {0} records processed. </t>
+  </si>
+  <si>
+    <t>https://online.immi.gov.au/lusc/login</t>
+  </si>
+  <si>
+    <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>Output_Header</t>
+  </si>
+  <si>
+    <t>EMPLID,FAMILY_NAME,GIVEN_NAMES,BIRTH_DATE,PASSPORT_NUMBER,PASSPORT_COUNTRY,LOCATION,UPDATETIMESTAMP,ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header fields for output file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email subject for error notification. </t>
+  </si>
+  <si>
+    <t>NoEmail_Message</t>
+  </si>
+  <si>
+    <t>Error message if no email or attachment found in mailbox</t>
+  </si>
+  <si>
+    <t>No new email or attachment found in mailbox to process.</t>
+  </si>
+  <si>
+    <t>OperatingEnvironment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot running environment </t>
+  </si>
+  <si>
+    <t>EmailMsg_InvalidCSV</t>
+  </si>
+  <si>
+    <t>Email message body if initialization error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message if move message to archive folder encounter error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if move invalid email (no attachment) to archive folder encounter error. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if error encountred while trying to read input CSV. </t>
+  </si>
+  <si>
+    <t>EmailMsg_InvalidEmail_MoveFolder</t>
+  </si>
+  <si>
+    <t>EmailMsg_NoAttachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email message body if no input csv attached to email </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error during Initialization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBI_LocationCheck process all records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error while trying to move email to archive folder.</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck encountered an error while trying to read input csv file.</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck process unable to process as bot didn't find input csv file 'EXTRACT_FOR_ROBOT.csv' in attachement.</t>
+  </si>
+  <si>
+    <t>RPA ADS support email address   -</t>
+  </si>
+  <si>
+    <t>rpa.ads@its.uq.edu.au</t>
+  </si>
+  <si>
+    <t>PBI_LocationCheck_AuthorisedSenderEmail</t>
+  </si>
+  <si>
     <t>Location VEVO check</t>
-  </si>
-  <si>
-    <t>Immi_Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder to save input file </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange server web address to retrive emails </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of emails to check (Top attribute in GetExchangeEmailessage activity) </t>
-  </si>
-  <si>
-    <t>Subject for email received from PBI team ro perform check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder to move email after processing </t>
-  </si>
-  <si>
-    <t>Credentials for SSO account  RPA00001</t>
-  </si>
-  <si>
-    <t>Credentials for Immi website login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBI team email address </t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck</t>
-  </si>
-  <si>
-    <t>Folder_Location</t>
-  </si>
-  <si>
-    <t>File_Name</t>
-  </si>
-  <si>
-    <t>EXTRACT_FOR_ROBOT.csv</t>
-  </si>
-  <si>
-    <t>File name for input, received from PBI team</t>
-  </si>
-  <si>
-    <t>Archive_Folder</t>
-  </si>
-  <si>
-    <t>PBI_Archive</t>
-  </si>
-  <si>
-    <t>Immi website (extrenal url)</t>
-  </si>
-  <si>
-    <t>Email_MessageBody</t>
-  </si>
-  <si>
-    <t>Email message body for response email</t>
-  </si>
-  <si>
-    <t>Email_AlertRecipient</t>
-  </si>
-  <si>
-    <t>Email_Alert_Subject</t>
-  </si>
-  <si>
-    <t>EmailMsg_MoveFolder</t>
-  </si>
-  <si>
-    <t>EmailMsg_InitError</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck - Error Notification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please find VEVO location check result attached. There are {0} records processed. </t>
-  </si>
-  <si>
-    <t>https://online.immi.gov.au/lusc/login</t>
-  </si>
-  <si>
-    <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
-  </si>
-  <si>
-    <t>Output_Header</t>
-  </si>
-  <si>
-    <t>EMPLID,FAMILY_NAME,GIVEN_NAMES,BIRTH_DATE,PASSPORT_NUMBER,PASSPORT_COUNTRY,LOCATION,UPDATETIMESTAMP,ERROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Header fields for output file </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email subject for error notification. </t>
-  </si>
-  <si>
-    <t>NoEmail_Message</t>
-  </si>
-  <si>
-    <t>Error message if no email or attachment found in mailbox</t>
-  </si>
-  <si>
-    <t>No new email or attachment found in mailbox to process.</t>
-  </si>
-  <si>
-    <t>OperatingEnvironment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robot running environment </t>
-  </si>
-  <si>
-    <t>EmailMsg_InvalidCSV</t>
-  </si>
-  <si>
-    <t>Email message body if initialization error.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email message if move message to archive folder encounter error. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email message body if move invalid email (no attachment) to archive folder encounter error. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email message body if error encountred while trying to read input CSV. </t>
-  </si>
-  <si>
-    <t>EmailMsg_InvalidEmail_MoveFolder</t>
-  </si>
-  <si>
-    <t>EmailMsg_NoAttachment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email message body if no input csv attached to email </t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck encountered an error during Initialization.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBI_LocationCheck process all records and sent updated file to PBI team however encountered an error while moving the email to ‘PBI_Archive’ folder which need manual intervention prior to next run. Kindly move email ‘{0}’ to PBI_Archive folder in RPA00001 Mailbox. </t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck encountered an error while trying to move email to archive folder.</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck encountered an error while trying to read input csv file.</t>
-  </si>
-  <si>
-    <t>PBI_LocationCheck process unable to process as bot didn't find input csv file 'EXTRACT_FOR_ROBOT.csv' in attachement.</t>
-  </si>
-  <si>
-    <t>RPA ADS support email address   -</t>
-  </si>
-  <si>
-    <t>rpa.ads@its.uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -703,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -752,35 +755,35 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -788,7 +791,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
@@ -800,10 +803,10 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -814,7 +817,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,33 +825,33 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1851,7 +1854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -2082,101 +2085,101 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
-      </c>
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
         <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
         <v>95</v>
-      </c>
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3159,7 +3162,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3209,7 +3212,7 @@
         <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3220,7 +3223,7 @@
         <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3228,21 +3231,21 @@
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
         <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>